<commit_message>
changed the matlab code to work on different pc's
</commit_message>
<xml_diff>
--- a/Stability/wind_tunnel_test/sample_data/wind_tunnel_measurement_data.xlsx
+++ b/Stability/wind_tunnel_test/sample_data/wind_tunnel_measurement_data.xlsx
@@ -13,7 +13,439 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_10_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_0_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_10_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_15_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_20_U_8_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_4_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_6_060623</t>
+  </si>
+  <si>
+    <t>M_10_setup5_aoa_5_U_8_060623</t>
+  </si>
+  <si>
+    <t>Mean Norm</t>
+  </si>
+  <si>
+    <t>Mean Ax</t>
+  </si>
   <si>
     <t>File Name</t>
   </si>
@@ -230,18 +662,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>196</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="B2" s="0">
         <v>-2.1052148335698173</v>
@@ -252,7 +684,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="B3" s="0">
         <v>-0.57895515931006769</v>
@@ -263,7 +695,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>183</v>
       </c>
       <c r="B4" s="0">
         <v>-1.287281973039589</v>
@@ -274,7 +706,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="B5" s="0">
         <v>-0.40182925073132802</v>
@@ -285,7 +717,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="B6" s="0">
         <v>-1.134549037892276</v>
@@ -296,7 +728,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="B7" s="0">
         <v>-2.3829568318191012</v>
@@ -307,7 +739,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="B8" s="0">
         <v>-0.42193840754912076</v>
@@ -318,7 +750,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="B9" s="0">
         <v>-1.3944283036287641</v>
@@ -329,7 +761,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="B10" s="0">
         <v>-2.803143165271063</v>
@@ -340,7 +772,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="B11" s="0">
         <v>-0.42784510148462046</v>
@@ -351,7 +783,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="B12" s="0">
         <v>-1.3001218445827887</v>
@@ -362,7 +794,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="B13" s="0">
         <v>-2.813494993779742</v>
@@ -373,7 +805,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="B14" s="0">
         <v>-0.30982714606405432</v>
@@ -384,7 +816,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="B15" s="0">
         <v>-0.91048429016526389</v>
@@ -395,7 +827,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
       <c r="B16" s="0">
         <v>-1.8988649206575541</v>

</xml_diff>